<commit_message>
thêm trường ngaythue vào table thuesanpham, tìm kiếm (biểu đồ) phần trăm thuesanpham từ ngày tháng năm và tìm kiếm (biểu đồ) doanh thu và số lượng đặt phòng, huỷ và chuyển phòng từ năm
</commit_message>
<xml_diff>
--- a/QuanLyKhachSan_MVC.NET/nhanViens.xlsx
+++ b/QuanLyKhachSan_MVC.NET/nhanViens.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -41,22 +41,16 @@
     <t xml:space="preserve">Chức vụ</t>
   </si>
   <si>
-    <t xml:space="preserve">Bộ phận</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vị trí bộ phận</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trạng thái</t>
   </si>
   <si>
-    <t xml:space="preserve">Võ Van Chính</t>
+    <t xml:space="preserve">Võ Văn Chính</t>
   </si>
   <si>
     <t xml:space="preserve">0373449865</t>
   </si>
   <si>
-    <t xml:space="preserve">Qu?ng Tr?-Tri?u Phong-Tri?u Ð?i</t>
+    <t xml:space="preserve">Quảng Trị-Triệu Phong-Triệu Đại</t>
   </si>
   <si>
     <t xml:space="preserve">123456789</t>
@@ -68,22 +62,34 @@
     <t xml:space="preserve">0001-01-01</t>
   </si>
   <si>
-    <t xml:space="preserve">còn làm vi?c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trần Khánh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">234585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tỉnh Lai Châu-Huyện Tam Đường-Xã Giang Ma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1233218</t>
+    <t xml:space="preserve">Hoạt động</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dụng Nguyễn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03256457895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tỉnh Tuyên Quang-Thành phố Tuyên Quang-Phường Nông Tiến</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245365875</t>
   </si>
   <si>
     <t xml:space="preserve">Đang hoạt động</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Khôi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tỉnh Lào Cai-Huyện Bát Xát-Xã A Mú Sung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123321562</t>
   </si>
 </sst>
 </file>
@@ -162,14 +168,8 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -177,151 +177,95 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
       <c r="L4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
         <v>21</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chỉnh sửa giao diện, chức năng thêm ảnh cho sản phẩm (dịch vụ)
</commit_message>
<xml_diff>
--- a/QuanLyKhachSan_MVC.NET/nhanViens.xlsx
+++ b/QuanLyKhachSan_MVC.NET/nhanViens.xlsx
@@ -65,31 +65,31 @@
     <t xml:space="preserve">Hoạt động</t>
   </si>
   <si>
-    <t xml:space="preserve">Dụng Nguyễn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03256457895</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tỉnh Tuyên Quang-Thành phố Tuyên Quang-Phường Nông Tiến</t>
-  </si>
-  <si>
-    <t xml:space="preserve">245365875</t>
+    <t xml:space="preserve">Nguyễn Khôi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tỉnh Cao Bằng-Huyện Bảo Lâm-Xã Vĩnh Quang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245236587</t>
   </si>
   <si>
     <t xml:space="preserve">Đang hoạt động</t>
   </si>
   <si>
-    <t xml:space="preserve">Nguyễn Khôi</t>
+    <t xml:space="preserve">Trần Khánh</t>
   </si>
   <si>
     <t xml:space="preserve">123456</t>
   </si>
   <si>
-    <t xml:space="preserve">Tỉnh Lào Cai-Huyện Bát Xát-Xã A Mú Sung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123321562</t>
+    <t xml:space="preserve">Tỉnh Hà Giang-Huyện Vị Xuyên-Thị trấn Nông Trường Việt Lâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123321658</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
chỉnh sửa giao diện chi tiết thuê phòng, xây dựng chức năng hiển thị số lượng sản phẩm ở biểu đồ trong là 5 và nhấn vào thì sẽ cộng lên 2, xoá các view mota
</commit_message>
<xml_diff>
--- a/QuanLyKhachSan_MVC.NET/nhanViens.xlsx
+++ b/QuanLyKhachSan_MVC.NET/nhanViens.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t xml:space="preserve">123469685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nam Lê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tỉnh Lai Châu-Huyện Than Uyên-Xã Pha Mu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123321576</t>
   </si>
 </sst>
 </file>
@@ -561,6 +570,38 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>